<commit_message>
Closed #97 - Finished work related to patient photo
</commit_message>
<xml_diff>
--- a/DatabaseUpdate/ExcelFiles/RelativeRelationshipConnections.xlsx
+++ b/DatabaseUpdate/ExcelFiles/RelativeRelationshipConnections.xlsx
@@ -421,7 +421,7 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:C14"/>
+  <x:dimension ref="A1:C16"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
@@ -581,6 +581,28 @@
         <x:v>18</x:v>
       </x:c>
     </x:row>
+    <x:row r="15" spans="1:3">
+      <x:c r="A15" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="B15" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="C15" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="16" spans="1:3">
+      <x:c r="A16" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="B16" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="C16" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+    </x:row>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>

</xml_diff>